<commit_message>
hecha actualizacion de estudiantes
</commit_message>
<xml_diff>
--- a/RA_SEPIA_V2 (5).xlsx
+++ b/RA_SEPIA_V2 (5).xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{7A8A4C94-5172-4DAE-8C22-2528B2F660F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BEAF297D-1266-46DD-937A-315E14D44D2A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F13110C-9039-4B97-BDBB-3CFBBBE4FEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="2160" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="117">
   <si>
     <r>
       <rPr>
@@ -382,12 +382,45 @@
   <si>
     <t>samuel julian cristian</t>
   </si>
+  <si>
+    <t>smartinezs2@correo.usbcali.edu.co</t>
+  </si>
+  <si>
+    <t>samymartsa123@gmail.com</t>
+  </si>
+  <si>
+    <t>SAMUEL MARTINEZ SANCHEZ</t>
+  </si>
+  <si>
+    <t>nabrilg2@correo.usbcali.edu.co</t>
+  </si>
+  <si>
+    <t>abril1gutierreznatalia@gmail.com</t>
+  </si>
+  <si>
+    <t>315/286-5504</t>
+  </si>
+  <si>
+    <t>NATALIA ABRIL GOMEZA</t>
+  </si>
+  <si>
+    <t>NATALIA ABRIL GOMEZE</t>
+  </si>
+  <si>
+    <t>315/286-5506</t>
+  </si>
+  <si>
+    <t>NATALIA ABRIL GOMEZI</t>
+  </si>
+  <si>
+    <t>abrilgutierrez1natalia@gmail.com</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -455,6 +488,13 @@
       <u/>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="6"/>
+      <color theme="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -584,7 +624,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -677,6 +717,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -695,19 +738,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" indent="77"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -722,54 +792,64 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" indent="77"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -861,9 +941,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -901,9 +981,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -936,26 +1016,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -988,26 +1051,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1181,13 +1227,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R99"/>
+  <dimension ref="A1:R107"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="104" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14:H16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A81" zoomScale="104" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G80" sqref="G80:G82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
     <col min="2" max="2" width="6.85546875" customWidth="1"/>
@@ -1208,233 +1254,233 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
+      <c r="A2" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="52" t="s">
+      <c r="A3" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E6" s="52" t="s">
+      <c r="E6" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E7" s="52" t="s">
+      <c r="E7" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="52"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E8" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
+      <c r="E8" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="54"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
-      <c r="M9" s="54"/>
-      <c r="N9" s="54"/>
-      <c r="O9" s="54"/>
-      <c r="P9" s="54"/>
-      <c r="Q9" s="54"/>
+      <c r="A9" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="43"/>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="43"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="55" t="s">
+      <c r="A10" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="55" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="55"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="55"/>
+      <c r="A11" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="45" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="56" t="s">
+      <c r="D12" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="57"/>
-      <c r="F12" s="60" t="s">
+      <c r="E12" s="48"/>
+      <c r="F12" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="47" t="s">
+      <c r="G12" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="60" t="s">
+      <c r="H12" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="56" t="s">
+      <c r="I12" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="57"/>
-      <c r="K12" s="43" t="s">
+      <c r="J12" s="48"/>
+      <c r="K12" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="44"/>
-      <c r="M12" s="47" t="s">
+      <c r="L12" s="54"/>
+      <c r="M12" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="N12" s="47" t="s">
+      <c r="N12" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="O12" s="43" t="s">
+      <c r="O12" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="P12" s="44"/>
+      <c r="P12" s="54"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="48"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="45"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="48"/>
-      <c r="O13" s="45"/>
-      <c r="P13" s="46"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="55"/>
+      <c r="L13" s="56"/>
+      <c r="M13" s="46"/>
+      <c r="N13" s="46"/>
+      <c r="O13" s="55"/>
+      <c r="P13" s="56"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
@@ -1459,8 +1505,8 @@
       <c r="H14" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="I14" s="32"/>
-      <c r="J14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="34"/>
       <c r="K14" s="14" t="s">
         <v>1</v>
       </c>
@@ -1487,8 +1533,8 @@
       <c r="F15" s="28"/>
       <c r="G15" s="25"/>
       <c r="H15" s="28"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="36"/>
       <c r="K15" s="16"/>
       <c r="L15" s="17"/>
       <c r="M15" s="12"/>
@@ -1507,8 +1553,8 @@
       <c r="F16" s="29"/>
       <c r="G16" s="26"/>
       <c r="H16" s="29"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="38"/>
       <c r="K16" s="18"/>
       <c r="L16" s="19"/>
       <c r="M16" s="13"/>
@@ -1530,7 +1576,7 @@
         <v>31</v>
       </c>
       <c r="E17" s="31"/>
-      <c r="F17" s="42" t="s">
+      <c r="F17" s="57" t="s">
         <v>32</v>
       </c>
       <c r="G17" s="24" t="s">
@@ -1539,8 +1585,8 @@
       <c r="H17" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="32"/>
-      <c r="J17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="34"/>
       <c r="K17" s="14" t="s">
         <v>1</v>
       </c>
@@ -1567,8 +1613,8 @@
       <c r="F18" s="28"/>
       <c r="G18" s="25"/>
       <c r="H18" s="28"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="36"/>
       <c r="K18" s="16"/>
       <c r="L18" s="17"/>
       <c r="M18" s="12"/>
@@ -1588,8 +1634,8 @@
       <c r="F19" s="29"/>
       <c r="G19" s="26"/>
       <c r="H19" s="29"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="38"/>
       <c r="K19" s="18"/>
       <c r="L19" s="19"/>
       <c r="M19" s="13"/>
@@ -1615,11 +1661,11 @@
       <c r="G20" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="I20" s="32"/>
-      <c r="J20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="34"/>
       <c r="K20" s="14" t="s">
         <v>1</v>
       </c>
@@ -1645,9 +1691,9 @@
       <c r="E21" s="21"/>
       <c r="F21" s="28"/>
       <c r="G21" s="25"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="35"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="36"/>
       <c r="K21" s="16"/>
       <c r="L21" s="17"/>
       <c r="M21" s="12"/>
@@ -1666,9 +1712,9 @@
       <c r="E22" s="23"/>
       <c r="F22" s="29"/>
       <c r="G22" s="26"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="37"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="38"/>
       <c r="K22" s="18"/>
       <c r="L22" s="19"/>
       <c r="M22" s="13"/>
@@ -1699,8 +1745,8 @@
       <c r="H23" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="I23" s="32"/>
-      <c r="J23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="34"/>
       <c r="K23" s="14" t="s">
         <v>1</v>
       </c>
@@ -1727,8 +1773,8 @@
       <c r="F24" s="28"/>
       <c r="G24" s="25"/>
       <c r="H24" s="28"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="36"/>
       <c r="K24" s="16"/>
       <c r="L24" s="17"/>
       <c r="M24" s="12"/>
@@ -1747,8 +1793,8 @@
       <c r="F25" s="29"/>
       <c r="G25" s="26"/>
       <c r="H25" s="29"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="38"/>
       <c r="K25" s="18"/>
       <c r="L25" s="19"/>
       <c r="M25" s="13"/>
@@ -1779,8 +1825,8 @@
       <c r="H26" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="I26" s="32"/>
-      <c r="J26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="34"/>
       <c r="K26" s="14" t="s">
         <v>1</v>
       </c>
@@ -1807,8 +1853,8 @@
       <c r="F27" s="28"/>
       <c r="G27" s="25"/>
       <c r="H27" s="28"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="36"/>
       <c r="K27" s="16"/>
       <c r="L27" s="17"/>
       <c r="M27" s="12"/>
@@ -1827,8 +1873,8 @@
       <c r="F28" s="29"/>
       <c r="G28" s="26"/>
       <c r="H28" s="29"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="38"/>
       <c r="K28" s="18"/>
       <c r="L28" s="19"/>
       <c r="M28" s="13"/>
@@ -1859,8 +1905,8 @@
       <c r="H29" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="I29" s="32"/>
-      <c r="J29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="34"/>
       <c r="K29" s="14" t="s">
         <v>1</v>
       </c>
@@ -1887,8 +1933,8 @@
       <c r="F30" s="28"/>
       <c r="G30" s="25"/>
       <c r="H30" s="28"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="35"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="36"/>
       <c r="K30" s="16"/>
       <c r="L30" s="17"/>
       <c r="M30" s="12"/>
@@ -1907,8 +1953,8 @@
       <c r="F31" s="29"/>
       <c r="G31" s="26"/>
       <c r="H31" s="29"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="38"/>
       <c r="K31" s="18"/>
       <c r="L31" s="19"/>
       <c r="M31" s="13"/>
@@ -1939,8 +1985,8 @@
       <c r="H32" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="I32" s="32"/>
-      <c r="J32" s="33"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="34"/>
       <c r="K32" s="14" t="s">
         <v>1</v>
       </c>
@@ -1967,8 +2013,8 @@
       <c r="F33" s="28"/>
       <c r="G33" s="25"/>
       <c r="H33" s="28"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="36"/>
       <c r="K33" s="16"/>
       <c r="L33" s="17"/>
       <c r="M33" s="12"/>
@@ -1987,8 +2033,8 @@
       <c r="F34" s="29"/>
       <c r="G34" s="26"/>
       <c r="H34" s="29"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="38"/>
       <c r="K34" s="18"/>
       <c r="L34" s="19"/>
       <c r="M34" s="13"/>
@@ -2019,8 +2065,8 @@
       <c r="H35" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="I35" s="32"/>
-      <c r="J35" s="33"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="34"/>
       <c r="K35" s="14" t="s">
         <v>1</v>
       </c>
@@ -2047,8 +2093,8 @@
       <c r="F36" s="28"/>
       <c r="G36" s="25"/>
       <c r="H36" s="28"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="35"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="36"/>
       <c r="K36" s="16"/>
       <c r="L36" s="17"/>
       <c r="M36" s="12"/>
@@ -2067,8 +2113,8 @@
       <c r="F37" s="29"/>
       <c r="G37" s="26"/>
       <c r="H37" s="29"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="38"/>
       <c r="K37" s="18"/>
       <c r="L37" s="19"/>
       <c r="M37" s="13"/>
@@ -2099,8 +2145,8 @@
       <c r="H38" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="I38" s="32"/>
-      <c r="J38" s="33"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="34"/>
       <c r="K38" s="14" t="s">
         <v>1</v>
       </c>
@@ -2127,8 +2173,8 @@
       <c r="F39" s="28"/>
       <c r="G39" s="25"/>
       <c r="H39" s="28"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="35"/>
+      <c r="I39" s="35"/>
+      <c r="J39" s="36"/>
       <c r="K39" s="16"/>
       <c r="L39" s="17"/>
       <c r="M39" s="12"/>
@@ -2147,8 +2193,8 @@
       <c r="F40" s="29"/>
       <c r="G40" s="26"/>
       <c r="H40" s="29"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="37"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="38"/>
       <c r="K40" s="18"/>
       <c r="L40" s="19"/>
       <c r="M40" s="13"/>
@@ -2179,8 +2225,8 @@
       <c r="H41" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="I41" s="32"/>
-      <c r="J41" s="33"/>
+      <c r="I41" s="33"/>
+      <c r="J41" s="34"/>
       <c r="K41" s="14" t="s">
         <v>1</v>
       </c>
@@ -2207,8 +2253,8 @@
       <c r="F42" s="28"/>
       <c r="G42" s="25"/>
       <c r="H42" s="28"/>
-      <c r="I42" s="34"/>
-      <c r="J42" s="35"/>
+      <c r="I42" s="35"/>
+      <c r="J42" s="36"/>
       <c r="K42" s="16"/>
       <c r="L42" s="17"/>
       <c r="M42" s="12"/>
@@ -2227,8 +2273,8 @@
       <c r="F43" s="29"/>
       <c r="G43" s="26"/>
       <c r="H43" s="29"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="37"/>
+      <c r="I43" s="37"/>
+      <c r="J43" s="38"/>
       <c r="K43" s="18"/>
       <c r="L43" s="19"/>
       <c r="M43" s="13"/>
@@ -2259,8 +2305,8 @@
       <c r="H44" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="I44" s="32"/>
-      <c r="J44" s="33"/>
+      <c r="I44" s="33"/>
+      <c r="J44" s="34"/>
       <c r="K44" s="14" t="s">
         <v>1</v>
       </c>
@@ -2287,8 +2333,8 @@
       <c r="F45" s="28"/>
       <c r="G45" s="25"/>
       <c r="H45" s="28"/>
-      <c r="I45" s="34"/>
-      <c r="J45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="36"/>
       <c r="K45" s="16"/>
       <c r="L45" s="17"/>
       <c r="M45" s="12"/>
@@ -2307,8 +2353,8 @@
       <c r="F46" s="29"/>
       <c r="G46" s="26"/>
       <c r="H46" s="29"/>
-      <c r="I46" s="36"/>
-      <c r="J46" s="37"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="38"/>
       <c r="K46" s="18"/>
       <c r="L46" s="19"/>
       <c r="M46" s="13"/>
@@ -2339,8 +2385,8 @@
       <c r="H47" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="I47" s="32"/>
-      <c r="J47" s="33"/>
+      <c r="I47" s="33"/>
+      <c r="J47" s="34"/>
       <c r="K47" s="14" t="s">
         <v>1</v>
       </c>
@@ -2367,8 +2413,8 @@
       <c r="F48" s="28"/>
       <c r="G48" s="25"/>
       <c r="H48" s="28"/>
-      <c r="I48" s="34"/>
-      <c r="J48" s="35"/>
+      <c r="I48" s="35"/>
+      <c r="J48" s="36"/>
       <c r="K48" s="16"/>
       <c r="L48" s="17"/>
       <c r="M48" s="12"/>
@@ -2387,8 +2433,8 @@
       <c r="F49" s="29"/>
       <c r="G49" s="26"/>
       <c r="H49" s="29"/>
-      <c r="I49" s="36"/>
-      <c r="J49" s="37"/>
+      <c r="I49" s="37"/>
+      <c r="J49" s="38"/>
       <c r="K49" s="18"/>
       <c r="L49" s="19"/>
       <c r="M49" s="13"/>
@@ -2416,11 +2462,11 @@
       <c r="G50" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="H50" s="49" t="s">
+      <c r="H50" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="I50" s="32"/>
-      <c r="J50" s="33"/>
+      <c r="I50" s="33"/>
+      <c r="J50" s="34"/>
       <c r="K50" s="14" t="s">
         <v>1</v>
       </c>
@@ -2447,8 +2493,8 @@
       <c r="F51" s="28"/>
       <c r="G51" s="25"/>
       <c r="H51" s="28"/>
-      <c r="I51" s="34"/>
-      <c r="J51" s="35"/>
+      <c r="I51" s="35"/>
+      <c r="J51" s="36"/>
       <c r="K51" s="16"/>
       <c r="L51" s="17"/>
       <c r="M51" s="12"/>
@@ -2467,8 +2513,8 @@
       <c r="F52" s="29"/>
       <c r="G52" s="26"/>
       <c r="H52" s="29"/>
-      <c r="I52" s="36"/>
-      <c r="J52" s="37"/>
+      <c r="I52" s="37"/>
+      <c r="J52" s="38"/>
       <c r="K52" s="18"/>
       <c r="L52" s="19"/>
       <c r="M52" s="13"/>
@@ -2496,11 +2542,11 @@
       <c r="G53" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="H53" s="49" t="s">
+      <c r="H53" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="I53" s="32"/>
-      <c r="J53" s="33"/>
+      <c r="I53" s="33"/>
+      <c r="J53" s="34"/>
       <c r="K53" s="14" t="s">
         <v>1</v>
       </c>
@@ -2527,8 +2573,8 @@
       <c r="F54" s="28"/>
       <c r="G54" s="25"/>
       <c r="H54" s="28"/>
-      <c r="I54" s="34"/>
-      <c r="J54" s="35"/>
+      <c r="I54" s="35"/>
+      <c r="J54" s="36"/>
       <c r="K54" s="16"/>
       <c r="L54" s="17"/>
       <c r="M54" s="12"/>
@@ -2547,8 +2593,8 @@
       <c r="F55" s="29"/>
       <c r="G55" s="26"/>
       <c r="H55" s="29"/>
-      <c r="I55" s="36"/>
-      <c r="J55" s="37"/>
+      <c r="I55" s="37"/>
+      <c r="J55" s="38"/>
       <c r="K55" s="18"/>
       <c r="L55" s="19"/>
       <c r="M55" s="13"/>
@@ -2579,8 +2625,8 @@
       <c r="H56" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="I56" s="32"/>
-      <c r="J56" s="33"/>
+      <c r="I56" s="33"/>
+      <c r="J56" s="34"/>
       <c r="K56" s="14" t="s">
         <v>1</v>
       </c>
@@ -2607,8 +2653,8 @@
       <c r="F57" s="28"/>
       <c r="G57" s="25"/>
       <c r="H57" s="28"/>
-      <c r="I57" s="34"/>
-      <c r="J57" s="35"/>
+      <c r="I57" s="35"/>
+      <c r="J57" s="36"/>
       <c r="K57" s="16"/>
       <c r="L57" s="17"/>
       <c r="M57" s="12"/>
@@ -2627,8 +2673,8 @@
       <c r="F58" s="29"/>
       <c r="G58" s="26"/>
       <c r="H58" s="29"/>
-      <c r="I58" s="36"/>
-      <c r="J58" s="37"/>
+      <c r="I58" s="37"/>
+      <c r="J58" s="38"/>
       <c r="K58" s="18"/>
       <c r="L58" s="19"/>
       <c r="M58" s="13"/>
@@ -2650,7 +2696,7 @@
         <v>31</v>
       </c>
       <c r="E59" s="31"/>
-      <c r="F59" s="42" t="s">
+      <c r="F59" s="57" t="s">
         <v>32</v>
       </c>
       <c r="G59" s="24" t="s">
@@ -2659,8 +2705,8 @@
       <c r="H59" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="I59" s="32"/>
-      <c r="J59" s="33"/>
+      <c r="I59" s="33"/>
+      <c r="J59" s="34"/>
       <c r="K59" s="14" t="s">
         <v>1</v>
       </c>
@@ -2687,8 +2733,8 @@
       <c r="F60" s="28"/>
       <c r="G60" s="25"/>
       <c r="H60" s="28"/>
-      <c r="I60" s="34"/>
-      <c r="J60" s="35"/>
+      <c r="I60" s="35"/>
+      <c r="J60" s="36"/>
       <c r="K60" s="16"/>
       <c r="L60" s="17"/>
       <c r="M60" s="12"/>
@@ -2707,8 +2753,8 @@
       <c r="F61" s="29"/>
       <c r="G61" s="26"/>
       <c r="H61" s="29"/>
-      <c r="I61" s="36"/>
-      <c r="J61" s="37"/>
+      <c r="I61" s="37"/>
+      <c r="J61" s="38"/>
       <c r="K61" s="18"/>
       <c r="L61" s="19"/>
       <c r="M61" s="13"/>
@@ -2717,8 +2763,8 @@
       <c r="P61" s="19"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" s="24" t="s">
-        <v>35</v>
+      <c r="A62" s="24">
+        <v>3</v>
       </c>
       <c r="B62" s="27" t="s">
         <v>36</v>
@@ -2734,11 +2780,11 @@
       <c r="G62" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="H62" s="38" t="s">
+      <c r="H62" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="I62" s="32"/>
-      <c r="J62" s="33"/>
+      <c r="I62" s="33"/>
+      <c r="J62" s="34"/>
       <c r="K62" s="14" t="s">
         <v>1</v>
       </c>
@@ -2764,9 +2810,9 @@
       <c r="E63" s="21"/>
       <c r="F63" s="28"/>
       <c r="G63" s="25"/>
-      <c r="H63" s="39"/>
-      <c r="I63" s="34"/>
-      <c r="J63" s="35"/>
+      <c r="H63" s="59"/>
+      <c r="I63" s="35"/>
+      <c r="J63" s="36"/>
       <c r="K63" s="16"/>
       <c r="L63" s="17"/>
       <c r="M63" s="12"/>
@@ -2784,9 +2830,9 @@
       <c r="E64" s="23"/>
       <c r="F64" s="29"/>
       <c r="G64" s="26"/>
-      <c r="H64" s="40"/>
-      <c r="I64" s="36"/>
-      <c r="J64" s="37"/>
+      <c r="H64" s="60"/>
+      <c r="I64" s="37"/>
+      <c r="J64" s="38"/>
       <c r="K64" s="18"/>
       <c r="L64" s="19"/>
       <c r="M64" s="13"/>
@@ -2817,8 +2863,8 @@
       <c r="H65" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="I65" s="32"/>
-      <c r="J65" s="33"/>
+      <c r="I65" s="33"/>
+      <c r="J65" s="34"/>
       <c r="K65" s="14" t="s">
         <v>1</v>
       </c>
@@ -2845,8 +2891,8 @@
       <c r="F66" s="28"/>
       <c r="G66" s="25"/>
       <c r="H66" s="28"/>
-      <c r="I66" s="34"/>
-      <c r="J66" s="35"/>
+      <c r="I66" s="35"/>
+      <c r="J66" s="36"/>
       <c r="K66" s="16"/>
       <c r="L66" s="17"/>
       <c r="M66" s="12"/>
@@ -2865,8 +2911,8 @@
       <c r="F67" s="29"/>
       <c r="G67" s="26"/>
       <c r="H67" s="29"/>
-      <c r="I67" s="36"/>
-      <c r="J67" s="37"/>
+      <c r="I67" s="37"/>
+      <c r="J67" s="38"/>
       <c r="K67" s="18"/>
       <c r="L67" s="19"/>
       <c r="M67" s="13"/>
@@ -2897,8 +2943,8 @@
       <c r="H68" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="I68" s="32"/>
-      <c r="J68" s="33"/>
+      <c r="I68" s="33"/>
+      <c r="J68" s="34"/>
       <c r="K68" s="14" t="s">
         <v>1</v>
       </c>
@@ -2925,8 +2971,8 @@
       <c r="F69" s="28"/>
       <c r="G69" s="25"/>
       <c r="H69" s="28"/>
-      <c r="I69" s="34"/>
-      <c r="J69" s="35"/>
+      <c r="I69" s="35"/>
+      <c r="J69" s="36"/>
       <c r="K69" s="16"/>
       <c r="L69" s="17"/>
       <c r="M69" s="12"/>
@@ -2945,8 +2991,8 @@
       <c r="F70" s="29"/>
       <c r="G70" s="26"/>
       <c r="H70" s="29"/>
-      <c r="I70" s="36"/>
-      <c r="J70" s="37"/>
+      <c r="I70" s="37"/>
+      <c r="J70" s="38"/>
       <c r="K70" s="18"/>
       <c r="L70" s="19"/>
       <c r="M70" s="13"/>
@@ -2977,8 +3023,8 @@
       <c r="H71" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="I71" s="32"/>
-      <c r="J71" s="33"/>
+      <c r="I71" s="33"/>
+      <c r="J71" s="34"/>
       <c r="K71" s="14" t="s">
         <v>1</v>
       </c>
@@ -3005,8 +3051,8 @@
       <c r="F72" s="28"/>
       <c r="G72" s="25"/>
       <c r="H72" s="28"/>
-      <c r="I72" s="34"/>
-      <c r="J72" s="35"/>
+      <c r="I72" s="35"/>
+      <c r="J72" s="36"/>
       <c r="K72" s="16"/>
       <c r="L72" s="17"/>
       <c r="M72" s="12"/>
@@ -3025,8 +3071,8 @@
       <c r="F73" s="29"/>
       <c r="G73" s="26"/>
       <c r="H73" s="29"/>
-      <c r="I73" s="36"/>
-      <c r="J73" s="37"/>
+      <c r="I73" s="37"/>
+      <c r="J73" s="38"/>
       <c r="K73" s="18"/>
       <c r="L73" s="19"/>
       <c r="M73" s="13"/>
@@ -3057,8 +3103,8 @@
       <c r="H74" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="I74" s="32"/>
-      <c r="J74" s="33"/>
+      <c r="I74" s="33"/>
+      <c r="J74" s="34"/>
       <c r="K74" s="14" t="s">
         <v>1</v>
       </c>
@@ -3085,8 +3131,8 @@
       <c r="F75" s="28"/>
       <c r="G75" s="25"/>
       <c r="H75" s="28"/>
-      <c r="I75" s="34"/>
-      <c r="J75" s="35"/>
+      <c r="I75" s="35"/>
+      <c r="J75" s="36"/>
       <c r="K75" s="16"/>
       <c r="L75" s="17"/>
       <c r="M75" s="12"/>
@@ -3105,8 +3151,8 @@
       <c r="F76" s="29"/>
       <c r="G76" s="26"/>
       <c r="H76" s="29"/>
-      <c r="I76" s="36"/>
-      <c r="J76" s="37"/>
+      <c r="I76" s="37"/>
+      <c r="J76" s="38"/>
       <c r="K76" s="18"/>
       <c r="L76" s="19"/>
       <c r="M76" s="13"/>
@@ -3137,8 +3183,8 @@
       <c r="H77" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="I77" s="32"/>
-      <c r="J77" s="33"/>
+      <c r="I77" s="33"/>
+      <c r="J77" s="34"/>
       <c r="K77" s="14" t="s">
         <v>1</v>
       </c>
@@ -3165,8 +3211,8 @@
       <c r="F78" s="28"/>
       <c r="G78" s="25"/>
       <c r="H78" s="28"/>
-      <c r="I78" s="34"/>
-      <c r="J78" s="35"/>
+      <c r="I78" s="35"/>
+      <c r="J78" s="36"/>
       <c r="K78" s="16"/>
       <c r="L78" s="17"/>
       <c r="M78" s="12"/>
@@ -3185,8 +3231,8 @@
       <c r="F79" s="29"/>
       <c r="G79" s="26"/>
       <c r="H79" s="29"/>
-      <c r="I79" s="36"/>
-      <c r="J79" s="37"/>
+      <c r="I79" s="37"/>
+      <c r="J79" s="38"/>
       <c r="K79" s="18"/>
       <c r="L79" s="19"/>
       <c r="M79" s="13"/>
@@ -3201,24 +3247,24 @@
       <c r="B80" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C80" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="D80" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="E80" s="31"/>
-      <c r="F80" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="G80" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="H80" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="I80" s="32"/>
-      <c r="J80" s="33"/>
+      <c r="C80" s="24">
+        <v>30000062842</v>
+      </c>
+      <c r="D80" s="69" t="s">
+        <v>106</v>
+      </c>
+      <c r="E80" s="62"/>
+      <c r="F80" s="70" t="s">
+        <v>107</v>
+      </c>
+      <c r="G80" s="71">
+        <v>3108437302</v>
+      </c>
+      <c r="H80" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="I80" s="33"/>
+      <c r="J80" s="34"/>
       <c r="K80" s="14" t="s">
         <v>1</v>
       </c>
@@ -3238,15 +3284,15 @@
       <c r="A81" s="25"/>
       <c r="B81" s="28"/>
       <c r="C81" s="25"/>
-      <c r="D81" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E81" s="21"/>
-      <c r="F81" s="28"/>
+      <c r="D81" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="E81" s="64"/>
+      <c r="F81" s="65"/>
       <c r="G81" s="25"/>
       <c r="H81" s="28"/>
-      <c r="I81" s="34"/>
-      <c r="J81" s="35"/>
+      <c r="I81" s="35"/>
+      <c r="J81" s="36"/>
       <c r="K81" s="16"/>
       <c r="L81" s="17"/>
       <c r="M81" s="12"/>
@@ -3258,15 +3304,15 @@
       <c r="A82" s="26"/>
       <c r="B82" s="29"/>
       <c r="C82" s="26"/>
-      <c r="D82" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E82" s="23"/>
-      <c r="F82" s="29"/>
+      <c r="D82" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="E82" s="67"/>
+      <c r="F82" s="68"/>
       <c r="G82" s="26"/>
       <c r="H82" s="29"/>
-      <c r="I82" s="36"/>
-      <c r="J82" s="37"/>
+      <c r="I82" s="37"/>
+      <c r="J82" s="38"/>
       <c r="K82" s="18"/>
       <c r="L82" s="19"/>
       <c r="M82" s="13"/>
@@ -3288,8 +3334,8 @@
         <v>81</v>
       </c>
       <c r="E83" s="31"/>
-      <c r="F83" s="27" t="s">
-        <v>82</v>
+      <c r="F83" s="57" t="s">
+        <v>116</v>
       </c>
       <c r="G83" s="24" t="s">
         <v>83</v>
@@ -3297,8 +3343,8 @@
       <c r="H83" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="I83" s="32"/>
-      <c r="J83" s="33"/>
+      <c r="I83" s="33"/>
+      <c r="J83" s="34"/>
       <c r="K83" s="14" t="s">
         <v>1</v>
       </c>
@@ -3325,8 +3371,8 @@
       <c r="F84" s="28"/>
       <c r="G84" s="25"/>
       <c r="H84" s="28"/>
-      <c r="I84" s="34"/>
-      <c r="J84" s="35"/>
+      <c r="I84" s="35"/>
+      <c r="J84" s="36"/>
       <c r="K84" s="16"/>
       <c r="L84" s="17"/>
       <c r="M84" s="12"/>
@@ -3345,8 +3391,8 @@
       <c r="F85" s="29"/>
       <c r="G85" s="26"/>
       <c r="H85" s="29"/>
-      <c r="I85" s="36"/>
-      <c r="J85" s="37"/>
+      <c r="I85" s="37"/>
+      <c r="J85" s="38"/>
       <c r="K85" s="18"/>
       <c r="L85" s="19"/>
       <c r="M85" s="13"/>
@@ -3354,165 +3400,334 @@
       <c r="O85" s="18"/>
       <c r="P85" s="19"/>
     </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A86" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B86" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C86" s="24">
+        <v>30000064302</v>
+      </c>
+      <c r="D86" s="61" t="s">
+        <v>109</v>
+      </c>
+      <c r="E86" s="31"/>
+      <c r="F86" s="57" t="s">
+        <v>110</v>
+      </c>
+      <c r="G86" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="H86" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="I86" s="33"/>
+      <c r="J86" s="34"/>
+      <c r="K86" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="L86" s="15"/>
+      <c r="M86" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N86" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="O86" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P86" s="15"/>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A87" s="25"/>
+      <c r="B87" s="28"/>
+      <c r="C87" s="25"/>
+      <c r="D87" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E87" s="21"/>
+      <c r="F87" s="28"/>
+      <c r="G87" s="25"/>
+      <c r="H87" s="28"/>
+      <c r="I87" s="35"/>
+      <c r="J87" s="36"/>
+      <c r="K87" s="16"/>
+      <c r="L87" s="17"/>
+      <c r="M87" s="12"/>
+      <c r="N87" s="12"/>
+      <c r="O87" s="16"/>
+      <c r="P87" s="17"/>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A88" s="26"/>
+      <c r="B88" s="29"/>
+      <c r="C88" s="26"/>
+      <c r="D88" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E88" s="23"/>
+      <c r="F88" s="29"/>
+      <c r="G88" s="26"/>
+      <c r="H88" s="29"/>
+      <c r="I88" s="37"/>
+      <c r="J88" s="38"/>
+      <c r="K88" s="18"/>
+      <c r="L88" s="19"/>
+      <c r="M88" s="13"/>
+      <c r="N88" s="13"/>
+      <c r="O88" s="18"/>
+      <c r="P88" s="19"/>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A89" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B89" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C89" s="24">
+        <v>30000064303</v>
+      </c>
+      <c r="D89" s="61" t="s">
+        <v>109</v>
+      </c>
+      <c r="E89" s="75"/>
+      <c r="F89" s="57" t="s">
+        <v>110</v>
+      </c>
+      <c r="G89" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="H89" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="I89" s="33"/>
+      <c r="J89" s="34"/>
+      <c r="K89" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="L89" s="15"/>
+      <c r="M89" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N89" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="O89" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P89" s="15"/>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A90" s="25"/>
+      <c r="B90" s="28"/>
+      <c r="C90" s="25"/>
+      <c r="D90" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E90" s="21"/>
+      <c r="F90" s="73"/>
+      <c r="G90" s="25"/>
+      <c r="H90" s="28"/>
+      <c r="I90" s="35"/>
+      <c r="J90" s="36"/>
+      <c r="K90" s="16"/>
+      <c r="L90" s="17"/>
+      <c r="M90" s="12"/>
+      <c r="N90" s="12"/>
+      <c r="O90" s="16"/>
+      <c r="P90" s="17"/>
+    </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A91" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="B91" s="41"/>
-      <c r="C91" s="41"/>
-      <c r="D91" s="41"/>
-      <c r="E91" s="41"/>
-      <c r="F91" s="41"/>
-      <c r="G91" s="41"/>
-      <c r="H91" s="41"/>
-      <c r="I91" s="41"/>
-      <c r="J91" s="41"/>
-      <c r="K91" s="41"/>
-      <c r="L91" s="41"/>
-      <c r="M91" s="41"/>
-      <c r="N91" s="41"/>
-      <c r="O91" s="41"/>
-      <c r="P91" s="41"/>
-      <c r="Q91" s="41"/>
+      <c r="A91" s="26"/>
+      <c r="B91" s="29"/>
+      <c r="C91" s="26"/>
+      <c r="D91" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E91" s="23"/>
+      <c r="F91" s="74"/>
+      <c r="G91" s="26"/>
+      <c r="H91" s="29"/>
+      <c r="I91" s="37"/>
+      <c r="J91" s="38"/>
+      <c r="K91" s="18"/>
+      <c r="L91" s="19"/>
+      <c r="M91" s="13"/>
+      <c r="N91" s="13"/>
+      <c r="O91" s="18"/>
+      <c r="P91" s="19"/>
+      <c r="Q91" s="72"/>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A92" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B92" s="3"/>
-      <c r="C92" s="3"/>
-      <c r="D92" s="3"/>
-      <c r="E92" s="3"/>
-      <c r="F92" s="3"/>
-      <c r="G92" s="10"/>
-      <c r="H92" s="3"/>
-      <c r="I92" s="3"/>
-      <c r="J92" s="3"/>
-      <c r="K92" s="3"/>
-      <c r="L92" s="3"/>
-      <c r="M92" s="3"/>
-      <c r="N92" s="3"/>
-      <c r="O92" s="3"/>
-      <c r="P92" s="3"/>
+      <c r="A92" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B92" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C92" s="24">
+        <v>30000064304</v>
+      </c>
+      <c r="D92" s="61" t="s">
+        <v>109</v>
+      </c>
+      <c r="E92" s="75"/>
+      <c r="F92" s="57" t="s">
+        <v>110</v>
+      </c>
+      <c r="G92" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="H92" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="I92" s="33"/>
+      <c r="J92" s="34"/>
+      <c r="K92" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="L92" s="15"/>
+      <c r="M92" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N92" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="O92" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P92" s="15"/>
       <c r="Q92" s="3"/>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A93" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B93" s="4"/>
-      <c r="C93" s="4"/>
-      <c r="D93" s="4"/>
-      <c r="E93" s="4"/>
-      <c r="F93" s="4"/>
-      <c r="G93" s="4"/>
-      <c r="H93" s="4"/>
-      <c r="I93" s="4"/>
-      <c r="J93" s="4"/>
-      <c r="K93" s="4"/>
-      <c r="L93" s="4"/>
-      <c r="M93" s="4"/>
-      <c r="N93" s="4"/>
-      <c r="O93" s="4"/>
-      <c r="P93" s="4"/>
+      <c r="A93" s="25"/>
+      <c r="B93" s="28"/>
+      <c r="C93" s="25"/>
+      <c r="D93" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E93" s="21"/>
+      <c r="F93" s="73"/>
+      <c r="G93" s="25"/>
+      <c r="H93" s="28"/>
+      <c r="I93" s="35"/>
+      <c r="J93" s="36"/>
+      <c r="K93" s="16"/>
+      <c r="L93" s="17"/>
+      <c r="M93" s="12"/>
+      <c r="N93" s="12"/>
+      <c r="O93" s="16"/>
+      <c r="P93" s="17"/>
       <c r="Q93" s="4"/>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B94" s="5"/>
-      <c r="C94" s="5"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="5"/>
-      <c r="F94" s="5"/>
-      <c r="G94" s="5"/>
-      <c r="H94" s="5"/>
-      <c r="I94" s="5"/>
-      <c r="J94" s="5"/>
-      <c r="K94" s="5"/>
-      <c r="L94" s="5"/>
-      <c r="M94" s="5"/>
-      <c r="N94" s="5"/>
-      <c r="O94" s="5"/>
-      <c r="P94" s="5"/>
+      <c r="A94" s="26"/>
+      <c r="B94" s="29"/>
+      <c r="C94" s="26"/>
+      <c r="D94" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E94" s="23"/>
+      <c r="F94" s="74"/>
+      <c r="G94" s="26"/>
+      <c r="H94" s="29"/>
+      <c r="I94" s="37"/>
+      <c r="J94" s="38"/>
+      <c r="K94" s="18"/>
+      <c r="L94" s="19"/>
+      <c r="M94" s="13"/>
+      <c r="N94" s="13"/>
+      <c r="O94" s="18"/>
+      <c r="P94" s="19"/>
       <c r="Q94" s="5"/>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A95" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B95" s="6"/>
-      <c r="C95" s="6"/>
-      <c r="D95" s="6"/>
-      <c r="E95" s="6"/>
-      <c r="F95" s="6"/>
-      <c r="G95" s="6"/>
-      <c r="H95" s="6"/>
-      <c r="I95" s="6"/>
-      <c r="J95" s="6"/>
-      <c r="K95" s="6"/>
-      <c r="L95" s="6"/>
-      <c r="M95" s="6"/>
-      <c r="N95" s="6"/>
-      <c r="O95" s="6"/>
-      <c r="P95" s="6"/>
+      <c r="A95" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B95" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C95" s="24">
+        <v>30000064305</v>
+      </c>
+      <c r="D95" s="61" t="s">
+        <v>109</v>
+      </c>
+      <c r="E95" s="75"/>
+      <c r="F95" s="57" t="s">
+        <v>110</v>
+      </c>
+      <c r="G95" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="H95" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="I95" s="33"/>
+      <c r="J95" s="34"/>
+      <c r="K95" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="L95" s="15"/>
+      <c r="M95" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N95" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="O95" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P95" s="15"/>
       <c r="Q95" s="6"/>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A96" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B96" s="6"/>
-      <c r="C96" s="6"/>
-      <c r="D96" s="6"/>
-      <c r="E96" s="6"/>
-      <c r="F96" s="6"/>
-      <c r="G96" s="6"/>
-      <c r="H96" s="6"/>
-      <c r="I96" s="6"/>
-      <c r="J96" s="6"/>
-      <c r="K96" s="6"/>
-      <c r="L96" s="6"/>
-      <c r="M96" s="6"/>
-      <c r="N96" s="6"/>
-      <c r="O96" s="6"/>
-      <c r="P96" s="6"/>
+      <c r="A96" s="25"/>
+      <c r="B96" s="28"/>
+      <c r="C96" s="25"/>
+      <c r="D96" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E96" s="21"/>
+      <c r="F96" s="73"/>
+      <c r="G96" s="25"/>
+      <c r="H96" s="28"/>
+      <c r="I96" s="35"/>
+      <c r="J96" s="36"/>
+      <c r="K96" s="16"/>
+      <c r="L96" s="17"/>
+      <c r="M96" s="12"/>
+      <c r="N96" s="12"/>
+      <c r="O96" s="16"/>
+      <c r="P96" s="17"/>
       <c r="Q96" s="6"/>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A97" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B97" s="6"/>
-      <c r="C97" s="6"/>
-      <c r="D97" s="6"/>
-      <c r="E97" s="6"/>
-      <c r="F97" s="6"/>
-      <c r="G97" s="6"/>
-      <c r="H97" s="6"/>
-      <c r="I97" s="6"/>
-      <c r="J97" s="6"/>
-      <c r="K97" s="6"/>
-      <c r="L97" s="6"/>
-      <c r="M97" s="6"/>
-      <c r="N97" s="6"/>
-      <c r="O97" s="6"/>
-      <c r="P97" s="6"/>
+      <c r="A97" s="26"/>
+      <c r="B97" s="29"/>
+      <c r="C97" s="26"/>
+      <c r="D97" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E97" s="23"/>
+      <c r="F97" s="74"/>
+      <c r="G97" s="26"/>
+      <c r="H97" s="29"/>
+      <c r="I97" s="37"/>
+      <c r="J97" s="38"/>
+      <c r="K97" s="18"/>
+      <c r="L97" s="19"/>
+      <c r="M97" s="13"/>
+      <c r="N97" s="13"/>
+      <c r="O97" s="18"/>
+      <c r="P97" s="19"/>
       <c r="Q97" s="6"/>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A98" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B98" s="7"/>
-      <c r="C98" s="7"/>
-      <c r="D98" s="7"/>
-      <c r="E98" s="7"/>
-      <c r="F98" s="7"/>
-      <c r="G98" s="7"/>
-      <c r="H98" s="7"/>
-      <c r="I98" s="7"/>
       <c r="J98" s="7"/>
       <c r="K98" s="7"/>
       <c r="L98" s="7"/>
@@ -3523,17 +3738,6 @@
       <c r="Q98" s="7"/>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A99" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="B99" s="8"/>
-      <c r="C99" s="8"/>
-      <c r="D99" s="8"/>
-      <c r="E99" s="8"/>
-      <c r="F99" s="8"/>
-      <c r="G99" s="8"/>
-      <c r="H99" s="8"/>
-      <c r="I99" s="8"/>
       <c r="J99" s="8"/>
       <c r="K99" s="8"/>
       <c r="L99" s="8"/>
@@ -3543,8 +3747,500 @@
       <c r="P99" s="8"/>
       <c r="Q99" s="8"/>
     </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+      <c r="G100" s="10"/>
+      <c r="H100" s="3"/>
+      <c r="I100" s="6"/>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4"/>
+      <c r="G101" s="4"/>
+      <c r="H101" s="4"/>
+      <c r="I101" s="6"/>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B102" s="5"/>
+      <c r="C102" s="5"/>
+      <c r="D102" s="5"/>
+      <c r="E102" s="5"/>
+      <c r="F102" s="5"/>
+      <c r="G102" s="5"/>
+      <c r="H102" s="5"/>
+      <c r="I102" s="7"/>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A103" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B103" s="6"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="8"/>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A104" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B104" s="6"/>
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="6"/>
+      <c r="H104" s="6"/>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A105" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B105" s="6"/>
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="6"/>
+      <c r="F105" s="6"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="6"/>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A106" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B106" s="7"/>
+      <c r="C106" s="7"/>
+      <c r="D106" s="7"/>
+      <c r="E106" s="7"/>
+      <c r="F106" s="7"/>
+      <c r="G106" s="7"/>
+      <c r="H106" s="7"/>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A107" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B107" s="8"/>
+      <c r="C107" s="8"/>
+      <c r="D107" s="8"/>
+      <c r="E107" s="8"/>
+      <c r="F107" s="8"/>
+      <c r="G107" s="8"/>
+      <c r="H107" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="361">
+  <mergeCells count="416">
+    <mergeCell ref="M92:M94"/>
+    <mergeCell ref="N92:N94"/>
+    <mergeCell ref="O92:P94"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="A95:A97"/>
+    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="C95:C97"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="F95:F97"/>
+    <mergeCell ref="G95:G97"/>
+    <mergeCell ref="H95:H97"/>
+    <mergeCell ref="I95:J97"/>
+    <mergeCell ref="K95:L97"/>
+    <mergeCell ref="M95:M97"/>
+    <mergeCell ref="N95:N97"/>
+    <mergeCell ref="O95:P97"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="A92:A94"/>
+    <mergeCell ref="B92:B94"/>
+    <mergeCell ref="C92:C94"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="F92:F94"/>
+    <mergeCell ref="G92:G94"/>
+    <mergeCell ref="H92:H94"/>
+    <mergeCell ref="I92:J94"/>
+    <mergeCell ref="K92:L94"/>
+    <mergeCell ref="M86:M88"/>
+    <mergeCell ref="N86:N88"/>
+    <mergeCell ref="O86:P88"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="A89:A91"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="C89:C91"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="F89:F91"/>
+    <mergeCell ref="G89:G91"/>
+    <mergeCell ref="H89:H91"/>
+    <mergeCell ref="I89:J91"/>
+    <mergeCell ref="K89:L91"/>
+    <mergeCell ref="M89:M91"/>
+    <mergeCell ref="N89:N91"/>
+    <mergeCell ref="O89:P91"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="A86:A88"/>
+    <mergeCell ref="B86:B88"/>
+    <mergeCell ref="C86:C88"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="F86:F88"/>
+    <mergeCell ref="G86:G88"/>
+    <mergeCell ref="H86:H88"/>
+    <mergeCell ref="I86:J88"/>
+    <mergeCell ref="K86:L88"/>
+    <mergeCell ref="M83:M85"/>
+    <mergeCell ref="N83:N85"/>
+    <mergeCell ref="O83:P85"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="F83:F85"/>
+    <mergeCell ref="G83:G85"/>
+    <mergeCell ref="H83:H85"/>
+    <mergeCell ref="I83:J85"/>
+    <mergeCell ref="K83:L85"/>
+    <mergeCell ref="M80:M82"/>
+    <mergeCell ref="N80:N82"/>
+    <mergeCell ref="O80:P82"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="A77:A79"/>
+    <mergeCell ref="B77:B79"/>
+    <mergeCell ref="C77:C79"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="F77:F79"/>
+    <mergeCell ref="A80:A82"/>
+    <mergeCell ref="B80:B82"/>
+    <mergeCell ref="C80:C82"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="F80:F82"/>
+    <mergeCell ref="G80:G82"/>
+    <mergeCell ref="H80:H82"/>
+    <mergeCell ref="I80:J82"/>
+    <mergeCell ref="K80:L82"/>
+    <mergeCell ref="G77:G79"/>
+    <mergeCell ref="H77:H79"/>
+    <mergeCell ref="I77:J79"/>
+    <mergeCell ref="K77:L79"/>
+    <mergeCell ref="M71:M73"/>
+    <mergeCell ref="N71:N73"/>
+    <mergeCell ref="O71:P73"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="M74:M76"/>
+    <mergeCell ref="N74:N76"/>
+    <mergeCell ref="O74:P76"/>
+    <mergeCell ref="M77:M79"/>
+    <mergeCell ref="N77:N79"/>
+    <mergeCell ref="O77:P79"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="B74:B76"/>
+    <mergeCell ref="C74:C76"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="F74:F76"/>
+    <mergeCell ref="G74:G76"/>
+    <mergeCell ref="H74:H76"/>
+    <mergeCell ref="I74:J76"/>
+    <mergeCell ref="K74:L76"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="C71:C73"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:F73"/>
+    <mergeCell ref="G71:G73"/>
+    <mergeCell ref="H71:H73"/>
+    <mergeCell ref="I71:J73"/>
+    <mergeCell ref="K71:L73"/>
+    <mergeCell ref="M68:M70"/>
+    <mergeCell ref="N68:N70"/>
+    <mergeCell ref="O68:P70"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="F65:F67"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="C68:C70"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="F68:F70"/>
+    <mergeCell ref="G68:G70"/>
+    <mergeCell ref="H68:H70"/>
+    <mergeCell ref="I68:J70"/>
+    <mergeCell ref="K68:L70"/>
+    <mergeCell ref="G65:G67"/>
+    <mergeCell ref="H65:H67"/>
+    <mergeCell ref="I65:J67"/>
+    <mergeCell ref="K65:L67"/>
+    <mergeCell ref="M59:M61"/>
+    <mergeCell ref="N59:N61"/>
+    <mergeCell ref="O59:P61"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="M62:M64"/>
+    <mergeCell ref="N62:N64"/>
+    <mergeCell ref="O62:P64"/>
+    <mergeCell ref="M65:M67"/>
+    <mergeCell ref="N65:N67"/>
+    <mergeCell ref="O65:P67"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="C62:C64"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="F62:F64"/>
+    <mergeCell ref="G62:G64"/>
+    <mergeCell ref="H62:H64"/>
+    <mergeCell ref="I62:J64"/>
+    <mergeCell ref="K62:L64"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="C56:C58"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="G56:G58"/>
+    <mergeCell ref="H56:H58"/>
+    <mergeCell ref="I56:J58"/>
+    <mergeCell ref="K56:L58"/>
+    <mergeCell ref="M56:M58"/>
+    <mergeCell ref="N56:N58"/>
+    <mergeCell ref="O56:P58"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:F61"/>
+    <mergeCell ref="G59:G61"/>
+    <mergeCell ref="H59:H61"/>
+    <mergeCell ref="I59:J61"/>
+    <mergeCell ref="K59:L61"/>
+    <mergeCell ref="M47:M49"/>
+    <mergeCell ref="N47:N49"/>
+    <mergeCell ref="O47:P49"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:F49"/>
+    <mergeCell ref="G47:G49"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="I47:J49"/>
+    <mergeCell ref="K47:L49"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="I44:J46"/>
+    <mergeCell ref="K44:L46"/>
+    <mergeCell ref="M38:M40"/>
+    <mergeCell ref="N38:N40"/>
+    <mergeCell ref="O38:P40"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="M41:M43"/>
+    <mergeCell ref="N41:N43"/>
+    <mergeCell ref="O41:P43"/>
+    <mergeCell ref="M44:M46"/>
+    <mergeCell ref="N44:N46"/>
+    <mergeCell ref="O44:P46"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="G41:G43"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="I41:J43"/>
+    <mergeCell ref="K41:L43"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="I38:J40"/>
+    <mergeCell ref="K38:L40"/>
+    <mergeCell ref="M35:M37"/>
+    <mergeCell ref="N35:N37"/>
+    <mergeCell ref="O35:P37"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="G35:G37"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="I35:J37"/>
+    <mergeCell ref="K35:L37"/>
+    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="I32:J34"/>
+    <mergeCell ref="K32:L34"/>
+    <mergeCell ref="M26:M28"/>
+    <mergeCell ref="N26:N28"/>
+    <mergeCell ref="O26:P28"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="M29:M31"/>
+    <mergeCell ref="N29:N31"/>
+    <mergeCell ref="O29:P31"/>
+    <mergeCell ref="M32:M34"/>
+    <mergeCell ref="N32:N34"/>
+    <mergeCell ref="O32:P34"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="I29:J31"/>
+    <mergeCell ref="K29:L31"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="I26:J28"/>
+    <mergeCell ref="K26:L28"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="M17:M19"/>
+    <mergeCell ref="N17:N19"/>
+    <mergeCell ref="O17:P19"/>
+    <mergeCell ref="M20:M22"/>
+    <mergeCell ref="N20:N22"/>
+    <mergeCell ref="O20:P22"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="M23:M25"/>
+    <mergeCell ref="N23:N25"/>
+    <mergeCell ref="O23:P25"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="I23:J25"/>
+    <mergeCell ref="K23:L25"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="I20:J22"/>
+    <mergeCell ref="K20:L22"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="I17:J19"/>
+    <mergeCell ref="K17:L19"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="K12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="O12:P13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="I14:J16"/>
+    <mergeCell ref="K14:L16"/>
+    <mergeCell ref="M14:M16"/>
+    <mergeCell ref="N14:N16"/>
+    <mergeCell ref="O14:P16"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="G50:G52"/>
+    <mergeCell ref="H50:H52"/>
+    <mergeCell ref="I50:J52"/>
+    <mergeCell ref="K50:L52"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A2:Q2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:K3"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="E4:K4"/>
+    <mergeCell ref="E5:K5"/>
+    <mergeCell ref="E6:K6"/>
+    <mergeCell ref="E7:K7"/>
+    <mergeCell ref="E8:K8"/>
+    <mergeCell ref="A9:Q9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:J13"/>
     <mergeCell ref="M50:M52"/>
     <mergeCell ref="N50:N52"/>
     <mergeCell ref="O50:P52"/>
@@ -3569,350 +4265,24 @@
     <mergeCell ref="C50:C52"/>
     <mergeCell ref="D50:E50"/>
     <mergeCell ref="F50:F52"/>
-    <mergeCell ref="G50:G52"/>
-    <mergeCell ref="H50:H52"/>
-    <mergeCell ref="I50:J52"/>
-    <mergeCell ref="K50:L52"/>
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="A2:Q2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:K3"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="E4:K4"/>
-    <mergeCell ref="E5:K5"/>
-    <mergeCell ref="E6:K6"/>
-    <mergeCell ref="E7:K7"/>
-    <mergeCell ref="E8:K8"/>
-    <mergeCell ref="A9:Q9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:J13"/>
-    <mergeCell ref="K12:L13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="O12:P13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="I14:J16"/>
-    <mergeCell ref="K14:L16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="I17:J19"/>
-    <mergeCell ref="K17:L19"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="M14:M16"/>
-    <mergeCell ref="N14:N16"/>
-    <mergeCell ref="O14:P16"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="M17:M19"/>
-    <mergeCell ref="N17:N19"/>
-    <mergeCell ref="O17:P19"/>
-    <mergeCell ref="M20:M22"/>
-    <mergeCell ref="N20:N22"/>
-    <mergeCell ref="O20:P22"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="M23:M25"/>
-    <mergeCell ref="N23:N25"/>
-    <mergeCell ref="O23:P25"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="G23:G25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="I23:J25"/>
-    <mergeCell ref="K23:L25"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="I20:J22"/>
-    <mergeCell ref="K20:L22"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="G26:G28"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="I26:J28"/>
-    <mergeCell ref="K26:L28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="I29:J31"/>
-    <mergeCell ref="K29:L31"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="M26:M28"/>
-    <mergeCell ref="N26:N28"/>
-    <mergeCell ref="O26:P28"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="M29:M31"/>
-    <mergeCell ref="N29:N31"/>
-    <mergeCell ref="O29:P31"/>
-    <mergeCell ref="M32:M34"/>
-    <mergeCell ref="N32:N34"/>
-    <mergeCell ref="O32:P34"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="M35:M37"/>
-    <mergeCell ref="N35:N37"/>
-    <mergeCell ref="O35:P37"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:F34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="G35:G37"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="I35:J37"/>
-    <mergeCell ref="K35:L37"/>
-    <mergeCell ref="G32:G34"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="I32:J34"/>
-    <mergeCell ref="K32:L34"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="I38:J40"/>
-    <mergeCell ref="K38:L40"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="G41:G43"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="I41:J43"/>
-    <mergeCell ref="K41:L43"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="M38:M40"/>
-    <mergeCell ref="N38:N40"/>
-    <mergeCell ref="O38:P40"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="M41:M43"/>
-    <mergeCell ref="N41:N43"/>
-    <mergeCell ref="O41:P43"/>
-    <mergeCell ref="M44:M46"/>
-    <mergeCell ref="N44:N46"/>
-    <mergeCell ref="O44:P46"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="M47:M49"/>
-    <mergeCell ref="N47:N49"/>
-    <mergeCell ref="O47:P49"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="F47:F49"/>
-    <mergeCell ref="G47:G49"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="I47:J49"/>
-    <mergeCell ref="K47:L49"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="I44:J46"/>
-    <mergeCell ref="K44:L46"/>
-    <mergeCell ref="A91:Q91"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="G56:G58"/>
-    <mergeCell ref="H56:H58"/>
-    <mergeCell ref="I56:J58"/>
-    <mergeCell ref="K56:L58"/>
-    <mergeCell ref="M56:M58"/>
-    <mergeCell ref="N56:N58"/>
-    <mergeCell ref="O56:P58"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F59:F61"/>
-    <mergeCell ref="G59:G61"/>
-    <mergeCell ref="H59:H61"/>
-    <mergeCell ref="I59:J61"/>
-    <mergeCell ref="K59:L61"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="C62:C64"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="F62:F64"/>
-    <mergeCell ref="G62:G64"/>
-    <mergeCell ref="H62:H64"/>
-    <mergeCell ref="I62:J64"/>
-    <mergeCell ref="K62:L64"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="G65:G67"/>
-    <mergeCell ref="H65:H67"/>
-    <mergeCell ref="I65:J67"/>
-    <mergeCell ref="K65:L67"/>
-    <mergeCell ref="M59:M61"/>
-    <mergeCell ref="N59:N61"/>
-    <mergeCell ref="O59:P61"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="M62:M64"/>
-    <mergeCell ref="N62:N64"/>
-    <mergeCell ref="O62:P64"/>
-    <mergeCell ref="M65:M67"/>
-    <mergeCell ref="N65:N67"/>
-    <mergeCell ref="O65:P67"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="F68:F70"/>
-    <mergeCell ref="G68:G70"/>
-    <mergeCell ref="H68:H70"/>
-    <mergeCell ref="I68:J70"/>
-    <mergeCell ref="K68:L70"/>
-    <mergeCell ref="M68:M70"/>
-    <mergeCell ref="N68:N70"/>
-    <mergeCell ref="O68:P70"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="F65:F67"/>
-    <mergeCell ref="A71:A73"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="C71:C73"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:F73"/>
-    <mergeCell ref="G71:G73"/>
-    <mergeCell ref="H71:H73"/>
-    <mergeCell ref="I71:J73"/>
-    <mergeCell ref="K71:L73"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="B74:B76"/>
-    <mergeCell ref="C74:C76"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="F74:F76"/>
-    <mergeCell ref="G74:G76"/>
-    <mergeCell ref="H74:H76"/>
-    <mergeCell ref="I74:J76"/>
-    <mergeCell ref="K74:L76"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="G77:G79"/>
-    <mergeCell ref="H77:H79"/>
-    <mergeCell ref="I77:J79"/>
-    <mergeCell ref="K77:L79"/>
-    <mergeCell ref="M71:M73"/>
-    <mergeCell ref="N71:N73"/>
-    <mergeCell ref="O71:P73"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="M74:M76"/>
-    <mergeCell ref="N74:N76"/>
-    <mergeCell ref="O74:P76"/>
-    <mergeCell ref="M77:M79"/>
-    <mergeCell ref="N77:N79"/>
-    <mergeCell ref="O77:P79"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="A80:A82"/>
-    <mergeCell ref="B80:B82"/>
-    <mergeCell ref="C80:C82"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="F80:F82"/>
-    <mergeCell ref="G80:G82"/>
-    <mergeCell ref="H80:H82"/>
-    <mergeCell ref="I80:J82"/>
-    <mergeCell ref="K80:L82"/>
-    <mergeCell ref="M80:M82"/>
-    <mergeCell ref="N80:N82"/>
-    <mergeCell ref="O80:P82"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="A77:A79"/>
-    <mergeCell ref="B77:B79"/>
-    <mergeCell ref="C77:C79"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="F77:F79"/>
-    <mergeCell ref="M83:M85"/>
-    <mergeCell ref="N83:N85"/>
-    <mergeCell ref="O83:P85"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="C83:C85"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="F83:F85"/>
-    <mergeCell ref="G83:G85"/>
-    <mergeCell ref="H83:H85"/>
-    <mergeCell ref="I83:J85"/>
-    <mergeCell ref="K83:L85"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F17" r:id="rId1" xr:uid="{4CE8D58B-08DA-4641-970F-DA3E06C92A09}"/>
     <hyperlink ref="F59" r:id="rId2" xr:uid="{0380BB9E-FB27-4A76-A11F-9128BBA63BAA}"/>
+    <hyperlink ref="D80" r:id="rId3" xr:uid="{CDD171E9-26BB-4C42-B3B6-F8D475EC97CA}"/>
+    <hyperlink ref="F80" r:id="rId4" xr:uid="{3A5A32EF-15F9-481B-8CC1-AD2EF9B0F931}"/>
+    <hyperlink ref="D86" r:id="rId5" xr:uid="{805D0E97-AE0D-4208-AFCC-61407B12DDF4}"/>
+    <hyperlink ref="F86" r:id="rId6" xr:uid="{CE744FAD-B126-4758-A250-52F0E22BDBDF}"/>
+    <hyperlink ref="F89" r:id="rId7" xr:uid="{D6B2B7F4-5B9B-41EB-8BDF-20FBF751A27E}"/>
+    <hyperlink ref="D89" r:id="rId8" xr:uid="{A5929FE7-DEE8-457D-9947-CF40D4AF8593}"/>
+    <hyperlink ref="F92" r:id="rId9" xr:uid="{0CBB4D81-3353-4814-876A-7EAF851DB8E0}"/>
+    <hyperlink ref="D92" r:id="rId10" xr:uid="{57413CBF-BF84-4531-A87D-12D44AB5F76D}"/>
+    <hyperlink ref="F95" r:id="rId11" xr:uid="{15F3981C-DD9A-47E2-B022-8D792D605FDC}"/>
+    <hyperlink ref="D95" r:id="rId12" xr:uid="{7DBF2E33-DE3C-4960-80F4-3429FD90464A}"/>
+    <hyperlink ref="F83" r:id="rId13" xr:uid="{E0C5142A-642D-4862-9ED7-13E7CB82DE03}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Merge branch 'samuel' into yulian"
This reverts commit c426150ae96e8ac70a96e089a1952de25847b57a, reversing
changes made to 1eddd40a9801676b95e0d3c7eb15e7eb201931b4.
</commit_message>
<xml_diff>
--- a/RA_SEPIA_V2 (5).xlsx
+++ b/RA_SEPIA_V2 (5).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F13110C-9039-4B97-BDBB-3CFBBBE4FEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF88C30-4CA6-4581-B765-5AA236581609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="110">
   <si>
     <r>
       <rPr>
@@ -383,44 +383,23 @@
     <t>samuel julian cristian</t>
   </si>
   <si>
-    <t>smartinezs2@correo.usbcali.edu.co</t>
-  </si>
-  <si>
-    <t>samymartsa123@gmail.com</t>
-  </si>
-  <si>
-    <t>SAMUEL MARTINEZ SANCHEZ</t>
-  </si>
-  <si>
     <t>nabrilg2@correo.usbcali.edu.co</t>
   </si>
   <si>
-    <t>abril1gutierreznatalia@gmail.com</t>
+    <t>abrilguti2erreznatalia@gmail.com</t>
   </si>
   <si>
     <t>315/286-5504</t>
   </si>
   <si>
-    <t>NATALIA ABRIL GOMEZA</t>
-  </si>
-  <si>
-    <t>NATALIA ABRIL GOMEZE</t>
-  </si>
-  <si>
-    <t>315/286-5506</t>
-  </si>
-  <si>
-    <t>NATALIA ABRIL GOMEZI</t>
-  </si>
-  <si>
-    <t>abrilgutierrez1natalia@gmail.com</t>
+    <t>NATALIA ABRIL GUTIERREZA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,13 +467,6 @@
       <u/>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="6"/>
-      <color theme="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -624,7 +596,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -804,47 +776,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1227,10 +1162,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R107"/>
+  <dimension ref="A1:R99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A81" zoomScale="104" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G80" sqref="G80:G82"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A79" zoomScale="104" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H86" sqref="H86:H88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2763,8 +2698,8 @@
       <c r="P61" s="19"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" s="24">
-        <v>3</v>
+      <c r="A62" s="24" t="s">
+        <v>35</v>
       </c>
       <c r="B62" s="27" t="s">
         <v>36</v>
@@ -3247,21 +3182,21 @@
       <c r="B80" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C80" s="24">
-        <v>30000062842</v>
-      </c>
-      <c r="D80" s="69" t="s">
-        <v>106</v>
-      </c>
-      <c r="E80" s="62"/>
-      <c r="F80" s="70" t="s">
-        <v>107</v>
-      </c>
-      <c r="G80" s="71">
-        <v>3108437302</v>
-      </c>
-      <c r="H80" s="32" t="s">
-        <v>108</v>
+      <c r="C80" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D80" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="E80" s="31"/>
+      <c r="F80" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="G80" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="H80" s="27" t="s">
+        <v>78</v>
       </c>
       <c r="I80" s="33"/>
       <c r="J80" s="34"/>
@@ -3284,11 +3219,11 @@
       <c r="A81" s="25"/>
       <c r="B81" s="28"/>
       <c r="C81" s="25"/>
-      <c r="D81" s="63" t="s">
-        <v>1</v>
-      </c>
-      <c r="E81" s="64"/>
-      <c r="F81" s="65"/>
+      <c r="D81" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E81" s="21"/>
+      <c r="F81" s="28"/>
       <c r="G81" s="25"/>
       <c r="H81" s="28"/>
       <c r="I81" s="35"/>
@@ -3304,11 +3239,11 @@
       <c r="A82" s="26"/>
       <c r="B82" s="29"/>
       <c r="C82" s="26"/>
-      <c r="D82" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="E82" s="67"/>
-      <c r="F82" s="68"/>
+      <c r="D82" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E82" s="23"/>
+      <c r="F82" s="29"/>
       <c r="G82" s="26"/>
       <c r="H82" s="29"/>
       <c r="I82" s="37"/>
@@ -3334,8 +3269,8 @@
         <v>81</v>
       </c>
       <c r="E83" s="31"/>
-      <c r="F83" s="57" t="s">
-        <v>116</v>
+      <c r="F83" s="27" t="s">
+        <v>82</v>
       </c>
       <c r="G83" s="24" t="s">
         <v>83</v>
@@ -3410,18 +3345,18 @@
       <c r="C86" s="24">
         <v>30000064302</v>
       </c>
-      <c r="D86" s="61" t="s">
-        <v>109</v>
+      <c r="D86" s="62" t="s">
+        <v>106</v>
       </c>
       <c r="E86" s="31"/>
       <c r="F86" s="57" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G86" s="24" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H86" s="27" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I86" s="33"/>
       <c r="J86" s="34"/>
@@ -3480,254 +3415,165 @@
       <c r="O88" s="18"/>
       <c r="P88" s="19"/>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A89" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="B89" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C89" s="24">
-        <v>30000064303</v>
-      </c>
-      <c r="D89" s="61" t="s">
-        <v>109</v>
-      </c>
-      <c r="E89" s="75"/>
-      <c r="F89" s="57" t="s">
-        <v>110</v>
-      </c>
-      <c r="G89" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="H89" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="I89" s="33"/>
-      <c r="J89" s="34"/>
-      <c r="K89" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="L89" s="15"/>
-      <c r="M89" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="N89" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="O89" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="P89" s="15"/>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A90" s="25"/>
-      <c r="B90" s="28"/>
-      <c r="C90" s="25"/>
-      <c r="D90" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E90" s="21"/>
-      <c r="F90" s="73"/>
-      <c r="G90" s="25"/>
-      <c r="H90" s="28"/>
-      <c r="I90" s="35"/>
-      <c r="J90" s="36"/>
-      <c r="K90" s="16"/>
-      <c r="L90" s="17"/>
-      <c r="M90" s="12"/>
-      <c r="N90" s="12"/>
-      <c r="O90" s="16"/>
-      <c r="P90" s="17"/>
-    </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A91" s="26"/>
-      <c r="B91" s="29"/>
-      <c r="C91" s="26"/>
-      <c r="D91" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E91" s="23"/>
-      <c r="F91" s="74"/>
-      <c r="G91" s="26"/>
-      <c r="H91" s="29"/>
-      <c r="I91" s="37"/>
-      <c r="J91" s="38"/>
-      <c r="K91" s="18"/>
-      <c r="L91" s="19"/>
-      <c r="M91" s="13"/>
-      <c r="N91" s="13"/>
-      <c r="O91" s="18"/>
-      <c r="P91" s="19"/>
-      <c r="Q91" s="72"/>
+      <c r="A91" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="B91" s="61"/>
+      <c r="C91" s="61"/>
+      <c r="D91" s="61"/>
+      <c r="E91" s="61"/>
+      <c r="F91" s="61"/>
+      <c r="G91" s="61"/>
+      <c r="H91" s="61"/>
+      <c r="I91" s="61"/>
+      <c r="J91" s="61"/>
+      <c r="K91" s="61"/>
+      <c r="L91" s="61"/>
+      <c r="M91" s="61"/>
+      <c r="N91" s="61"/>
+      <c r="O91" s="61"/>
+      <c r="P91" s="61"/>
+      <c r="Q91" s="61"/>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A92" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="B92" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C92" s="24">
-        <v>30000064304</v>
-      </c>
-      <c r="D92" s="61" t="s">
-        <v>109</v>
-      </c>
-      <c r="E92" s="75"/>
-      <c r="F92" s="57" t="s">
-        <v>110</v>
-      </c>
-      <c r="G92" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="H92" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="I92" s="33"/>
-      <c r="J92" s="34"/>
-      <c r="K92" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="L92" s="15"/>
-      <c r="M92" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="N92" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="O92" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="P92" s="15"/>
+      <c r="A92" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="10"/>
+      <c r="H92" s="3"/>
+      <c r="I92" s="3"/>
+      <c r="J92" s="3"/>
+      <c r="K92" s="3"/>
+      <c r="L92" s="3"/>
+      <c r="M92" s="3"/>
+      <c r="N92" s="3"/>
+      <c r="O92" s="3"/>
+      <c r="P92" s="3"/>
       <c r="Q92" s="3"/>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A93" s="25"/>
-      <c r="B93" s="28"/>
-      <c r="C93" s="25"/>
-      <c r="D93" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E93" s="21"/>
-      <c r="F93" s="73"/>
-      <c r="G93" s="25"/>
-      <c r="H93" s="28"/>
-      <c r="I93" s="35"/>
-      <c r="J93" s="36"/>
-      <c r="K93" s="16"/>
-      <c r="L93" s="17"/>
-      <c r="M93" s="12"/>
-      <c r="N93" s="12"/>
-      <c r="O93" s="16"/>
-      <c r="P93" s="17"/>
+      <c r="A93" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="4"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="4"/>
+      <c r="J93" s="4"/>
+      <c r="K93" s="4"/>
+      <c r="L93" s="4"/>
+      <c r="M93" s="4"/>
+      <c r="N93" s="4"/>
+      <c r="O93" s="4"/>
+      <c r="P93" s="4"/>
       <c r="Q93" s="4"/>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A94" s="26"/>
-      <c r="B94" s="29"/>
-      <c r="C94" s="26"/>
-      <c r="D94" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E94" s="23"/>
-      <c r="F94" s="74"/>
-      <c r="G94" s="26"/>
-      <c r="H94" s="29"/>
-      <c r="I94" s="37"/>
-      <c r="J94" s="38"/>
-      <c r="K94" s="18"/>
-      <c r="L94" s="19"/>
-      <c r="M94" s="13"/>
-      <c r="N94" s="13"/>
-      <c r="O94" s="18"/>
-      <c r="P94" s="19"/>
+      <c r="A94" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5"/>
+      <c r="H94" s="5"/>
+      <c r="I94" s="5"/>
+      <c r="J94" s="5"/>
+      <c r="K94" s="5"/>
+      <c r="L94" s="5"/>
+      <c r="M94" s="5"/>
+      <c r="N94" s="5"/>
+      <c r="O94" s="5"/>
+      <c r="P94" s="5"/>
       <c r="Q94" s="5"/>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A95" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="B95" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C95" s="24">
-        <v>30000064305</v>
-      </c>
-      <c r="D95" s="61" t="s">
-        <v>109</v>
-      </c>
-      <c r="E95" s="75"/>
-      <c r="F95" s="57" t="s">
-        <v>110</v>
-      </c>
-      <c r="G95" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="H95" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="I95" s="33"/>
-      <c r="J95" s="34"/>
-      <c r="K95" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="L95" s="15"/>
-      <c r="M95" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="N95" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="O95" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="P95" s="15"/>
+      <c r="A95" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B95" s="6"/>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="6"/>
+      <c r="J95" s="6"/>
+      <c r="K95" s="6"/>
+      <c r="L95" s="6"/>
+      <c r="M95" s="6"/>
+      <c r="N95" s="6"/>
+      <c r="O95" s="6"/>
+      <c r="P95" s="6"/>
       <c r="Q95" s="6"/>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A96" s="25"/>
-      <c r="B96" s="28"/>
-      <c r="C96" s="25"/>
-      <c r="D96" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E96" s="21"/>
-      <c r="F96" s="73"/>
-      <c r="G96" s="25"/>
-      <c r="H96" s="28"/>
-      <c r="I96" s="35"/>
-      <c r="J96" s="36"/>
-      <c r="K96" s="16"/>
-      <c r="L96" s="17"/>
-      <c r="M96" s="12"/>
-      <c r="N96" s="12"/>
-      <c r="O96" s="16"/>
-      <c r="P96" s="17"/>
+      <c r="A96" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B96" s="6"/>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+      <c r="J96" s="6"/>
+      <c r="K96" s="6"/>
+      <c r="L96" s="6"/>
+      <c r="M96" s="6"/>
+      <c r="N96" s="6"/>
+      <c r="O96" s="6"/>
+      <c r="P96" s="6"/>
       <c r="Q96" s="6"/>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A97" s="26"/>
-      <c r="B97" s="29"/>
-      <c r="C97" s="26"/>
-      <c r="D97" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E97" s="23"/>
-      <c r="F97" s="74"/>
-      <c r="G97" s="26"/>
-      <c r="H97" s="29"/>
-      <c r="I97" s="37"/>
-      <c r="J97" s="38"/>
-      <c r="K97" s="18"/>
-      <c r="L97" s="19"/>
-      <c r="M97" s="13"/>
-      <c r="N97" s="13"/>
-      <c r="O97" s="18"/>
-      <c r="P97" s="19"/>
+      <c r="A97" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B97" s="6"/>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
+      <c r="G97" s="6"/>
+      <c r="H97" s="6"/>
+      <c r="I97" s="6"/>
+      <c r="J97" s="6"/>
+      <c r="K97" s="6"/>
+      <c r="L97" s="6"/>
+      <c r="M97" s="6"/>
+      <c r="N97" s="6"/>
+      <c r="O97" s="6"/>
+      <c r="P97" s="6"/>
       <c r="Q97" s="6"/>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A98" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B98" s="7"/>
+      <c r="C98" s="7"/>
+      <c r="D98" s="7"/>
+      <c r="E98" s="7"/>
+      <c r="F98" s="7"/>
+      <c r="G98" s="7"/>
+      <c r="H98" s="7"/>
+      <c r="I98" s="7"/>
       <c r="J98" s="7"/>
       <c r="K98" s="7"/>
       <c r="L98" s="7"/>
@@ -3738,6 +3584,17 @@
       <c r="Q98" s="7"/>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A99" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B99" s="8"/>
+      <c r="C99" s="8"/>
+      <c r="D99" s="8"/>
+      <c r="E99" s="8"/>
+      <c r="F99" s="8"/>
+      <c r="G99" s="8"/>
+      <c r="H99" s="8"/>
+      <c r="I99" s="8"/>
       <c r="J99" s="8"/>
       <c r="K99" s="8"/>
       <c r="L99" s="8"/>
@@ -3747,155 +3604,13 @@
       <c r="P99" s="8"/>
       <c r="Q99" s="8"/>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A100" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B100" s="3"/>
-      <c r="C100" s="3"/>
-      <c r="D100" s="3"/>
-      <c r="E100" s="3"/>
-      <c r="F100" s="3"/>
-      <c r="G100" s="10"/>
-      <c r="H100" s="3"/>
-      <c r="I100" s="6"/>
-    </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A101" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B101" s="4"/>
-      <c r="C101" s="4"/>
-      <c r="D101" s="4"/>
-      <c r="E101" s="4"/>
-      <c r="F101" s="4"/>
-      <c r="G101" s="4"/>
-      <c r="H101" s="4"/>
-      <c r="I101" s="6"/>
-    </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A102" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B102" s="5"/>
-      <c r="C102" s="5"/>
-      <c r="D102" s="5"/>
-      <c r="E102" s="5"/>
-      <c r="F102" s="5"/>
-      <c r="G102" s="5"/>
-      <c r="H102" s="5"/>
-      <c r="I102" s="7"/>
-    </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A103" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B103" s="6"/>
-      <c r="C103" s="6"/>
-      <c r="D103" s="6"/>
-      <c r="E103" s="6"/>
-      <c r="F103" s="6"/>
-      <c r="G103" s="6"/>
-      <c r="H103" s="6"/>
-      <c r="I103" s="8"/>
-    </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A104" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B104" s="6"/>
-      <c r="C104" s="6"/>
-      <c r="D104" s="6"/>
-      <c r="E104" s="6"/>
-      <c r="F104" s="6"/>
-      <c r="G104" s="6"/>
-      <c r="H104" s="6"/>
-    </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A105" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B105" s="6"/>
-      <c r="C105" s="6"/>
-      <c r="D105" s="6"/>
-      <c r="E105" s="6"/>
-      <c r="F105" s="6"/>
-      <c r="G105" s="6"/>
-      <c r="H105" s="6"/>
-    </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A106" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B106" s="7"/>
-      <c r="C106" s="7"/>
-      <c r="D106" s="7"/>
-      <c r="E106" s="7"/>
-      <c r="F106" s="7"/>
-      <c r="G106" s="7"/>
-      <c r="H106" s="7"/>
-    </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A107" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="B107" s="8"/>
-      <c r="C107" s="8"/>
-      <c r="D107" s="8"/>
-      <c r="E107" s="8"/>
-      <c r="F107" s="8"/>
-      <c r="G107" s="8"/>
-      <c r="H107" s="8"/>
-    </row>
   </sheetData>
-  <mergeCells count="416">
-    <mergeCell ref="M92:M94"/>
-    <mergeCell ref="N92:N94"/>
-    <mergeCell ref="O92:P94"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="A95:A97"/>
-    <mergeCell ref="B95:B97"/>
-    <mergeCell ref="C95:C97"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="F95:F97"/>
-    <mergeCell ref="G95:G97"/>
-    <mergeCell ref="H95:H97"/>
-    <mergeCell ref="I95:J97"/>
-    <mergeCell ref="K95:L97"/>
-    <mergeCell ref="M95:M97"/>
-    <mergeCell ref="N95:N97"/>
-    <mergeCell ref="O95:P97"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="A92:A94"/>
-    <mergeCell ref="B92:B94"/>
-    <mergeCell ref="C92:C94"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="F92:F94"/>
-    <mergeCell ref="G92:G94"/>
-    <mergeCell ref="H92:H94"/>
-    <mergeCell ref="I92:J94"/>
-    <mergeCell ref="K92:L94"/>
+  <mergeCells count="375">
     <mergeCell ref="M86:M88"/>
     <mergeCell ref="N86:N88"/>
     <mergeCell ref="O86:P88"/>
     <mergeCell ref="D87:E87"/>
     <mergeCell ref="D88:E88"/>
-    <mergeCell ref="A89:A91"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="C89:C91"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="F89:F91"/>
-    <mergeCell ref="G89:G91"/>
-    <mergeCell ref="H89:H91"/>
-    <mergeCell ref="I89:J91"/>
-    <mergeCell ref="K89:L91"/>
-    <mergeCell ref="M89:M91"/>
-    <mergeCell ref="N89:N91"/>
-    <mergeCell ref="O89:P91"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D91:E91"/>
     <mergeCell ref="A86:A88"/>
     <mergeCell ref="B86:B88"/>
     <mergeCell ref="C86:C88"/>
@@ -4022,6 +3737,7 @@
     <mergeCell ref="K62:L64"/>
     <mergeCell ref="D63:E63"/>
     <mergeCell ref="D64:E64"/>
+    <mergeCell ref="A91:Q91"/>
     <mergeCell ref="A56:A58"/>
     <mergeCell ref="B56:B58"/>
     <mergeCell ref="C56:C58"/>
@@ -4269,20 +3985,11 @@
   <hyperlinks>
     <hyperlink ref="F17" r:id="rId1" xr:uid="{4CE8D58B-08DA-4641-970F-DA3E06C92A09}"/>
     <hyperlink ref="F59" r:id="rId2" xr:uid="{0380BB9E-FB27-4A76-A11F-9128BBA63BAA}"/>
-    <hyperlink ref="D80" r:id="rId3" xr:uid="{CDD171E9-26BB-4C42-B3B6-F8D475EC97CA}"/>
-    <hyperlink ref="F80" r:id="rId4" xr:uid="{3A5A32EF-15F9-481B-8CC1-AD2EF9B0F931}"/>
-    <hyperlink ref="D86" r:id="rId5" xr:uid="{805D0E97-AE0D-4208-AFCC-61407B12DDF4}"/>
-    <hyperlink ref="F86" r:id="rId6" xr:uid="{CE744FAD-B126-4758-A250-52F0E22BDBDF}"/>
-    <hyperlink ref="F89" r:id="rId7" xr:uid="{D6B2B7F4-5B9B-41EB-8BDF-20FBF751A27E}"/>
-    <hyperlink ref="D89" r:id="rId8" xr:uid="{A5929FE7-DEE8-457D-9947-CF40D4AF8593}"/>
-    <hyperlink ref="F92" r:id="rId9" xr:uid="{0CBB4D81-3353-4814-876A-7EAF851DB8E0}"/>
-    <hyperlink ref="D92" r:id="rId10" xr:uid="{57413CBF-BF84-4531-A87D-12D44AB5F76D}"/>
-    <hyperlink ref="F95" r:id="rId11" xr:uid="{15F3981C-DD9A-47E2-B022-8D792D605FDC}"/>
-    <hyperlink ref="D95" r:id="rId12" xr:uid="{7DBF2E33-DE3C-4960-80F4-3429FD90464A}"/>
-    <hyperlink ref="F83" r:id="rId13" xr:uid="{E0C5142A-642D-4862-9ED7-13E7CB82DE03}"/>
+    <hyperlink ref="D86" r:id="rId3" xr:uid="{ADA8BD6A-9E35-43BF-8A19-CE6020A2D99D}"/>
+    <hyperlink ref="F86" r:id="rId4" xr:uid="{E6F36681-D3BA-44F7-A872-55AA974A5265}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
-  <drawing r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>